<commit_message>
Adding new Test Cases
</commit_message>
<xml_diff>
--- a/src/test/resources/DataStorage/TestData.xlsx
+++ b/src/test/resources/DataStorage/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SecurianAutomationProject\SecurianAutomationProject\src\test\resources\DataStorage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\SecurianAutomationProject\src\test\resources\DataStorage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF3F5F3E-6C6F-4709-ADE8-269742CC1E0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A4E326-9CA6-4CF7-99EC-E2C817D7D20D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8B8641E2-D680-4C78-A58D-91959C674F7B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{8B8641E2-D680-4C78-A58D-91959C674F7B}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -85,6 +85,24 @@
   </si>
   <si>
     <t>Congratulations! You are exceeding your retirement goals</t>
+  </si>
+  <si>
+    <t>TC_02</t>
+  </si>
+  <si>
+    <t>Mandatory Field Error Test</t>
+  </si>
+  <si>
+    <t>ErrorMsg</t>
+  </si>
+  <si>
+    <t>FieldErrorMsg</t>
+  </si>
+  <si>
+    <t>Please fill out all required fields</t>
+  </si>
+  <si>
+    <t>Input required</t>
   </si>
 </sst>
 </file>
@@ -436,33 +454,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7154C20-1911-4326-8593-71D7C9ED3E85}">
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:U4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" customWidth="1"/>
-    <col min="2" max="2" width="26.44140625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="17.5546875" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" customWidth="1"/>
+    <col min="2" max="2" width="26.453125" customWidth="1"/>
+    <col min="3" max="3" width="15.6328125" customWidth="1"/>
+    <col min="4" max="4" width="17.54296875" customWidth="1"/>
+    <col min="5" max="5" width="15.453125" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="21.109375" customWidth="1"/>
-    <col min="8" max="8" width="19.5546875" customWidth="1"/>
-    <col min="9" max="9" width="20.5546875" customWidth="1"/>
-    <col min="10" max="10" width="20.88671875" customWidth="1"/>
-    <col min="11" max="11" width="18.44140625" customWidth="1"/>
-    <col min="12" max="12" width="17.77734375" customWidth="1"/>
-    <col min="13" max="13" width="23.6640625" customWidth="1"/>
-    <col min="14" max="14" width="18.21875" customWidth="1"/>
-    <col min="15" max="15" width="19.5546875" customWidth="1"/>
-    <col min="16" max="16" width="51" customWidth="1"/>
+    <col min="7" max="7" width="21.08984375" customWidth="1"/>
+    <col min="8" max="8" width="19.54296875" customWidth="1"/>
+    <col min="9" max="9" width="20.54296875" customWidth="1"/>
+    <col min="10" max="10" width="20.90625" customWidth="1"/>
+    <col min="11" max="11" width="18.453125" customWidth="1"/>
+    <col min="12" max="12" width="17.81640625" customWidth="1"/>
+    <col min="13" max="13" width="23.6328125" customWidth="1"/>
+    <col min="14" max="14" width="18.1796875" customWidth="1"/>
+    <col min="15" max="15" width="19.54296875" customWidth="1"/>
+    <col min="16" max="16" width="38.36328125" customWidth="1"/>
+    <col min="17" max="17" width="29.6328125" customWidth="1"/>
+    <col min="18" max="18" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -511,11 +531,17 @@
       <c r="P1" t="s">
         <v>18</v>
       </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>23</v>
+      </c>
       <c r="U1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -563,9 +589,63 @@
       </c>
       <c r="P2" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4">
+        <v>68</v>
+      </c>
+      <c r="E4">
+        <v>100000</v>
+      </c>
+      <c r="F4">
+        <v>75000</v>
+      </c>
+      <c r="G4">
+        <v>500000</v>
+      </c>
+      <c r="H4">
+        <v>10</v>
+      </c>
+      <c r="I4">
+        <v>25</v>
+      </c>
+      <c r="J4">
+        <v>4000</v>
+      </c>
+      <c r="K4">
+        <v>500</v>
+      </c>
+      <c r="L4">
+        <v>20</v>
+      </c>
+      <c r="M4">
+        <v>75</v>
+      </c>
+      <c r="N4">
+        <v>8</v>
+      </c>
+      <c r="O4">
+        <v>5</v>
+      </c>
+      <c r="P4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>24</v>
+      </c>
+      <c r="R4" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>